<commit_message>
change part number for LDO in BOM. update PCB. script for generating gerbers
</commit_message>
<xml_diff>
--- a/v2/BOM/bluzDK_bom.xlsx
+++ b/v2/BOM/bluzDK_bom.xlsx
@@ -120,9 +120,6 @@
     <t>ABS06-32.768KHZ-9-T</t>
   </si>
   <si>
-    <t>AP2127K-3.3TRG1</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>SOIC-8</t>
   </si>
   <si>
-    <t>Diodes</t>
-  </si>
-  <si>
     <t>32.768KHz</t>
   </si>
   <si>
@@ -192,7 +186,13 @@
     <t>2Mb</t>
   </si>
   <si>
-    <t>SOT-23</t>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>MCP1700T-3302E/TT</t>
   </si>
 </sst>
 </file>
@@ -311,16 +311,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -685,13 +682,13 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
@@ -703,32 +700,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -736,360 +733,360 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="12">
+      <c r="H2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="11">
         <v>1</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="F3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="F5" s="11"/>
+      <c r="G5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11">
+        <v>3</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="11">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11">
+        <v>6</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="11">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="11">
         <v>1</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="12">
-        <v>3</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="F11" s="11"/>
+      <c r="G11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="F12" s="11"/>
+      <c r="G12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="11">
         <v>2</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="12">
-        <v>6</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="12">
-        <v>2</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="12">
-        <v>1</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="12">
-        <v>2</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+      <c r="H13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14">
       <c r="J15"/>
@@ -1104,15 +1101,15 @@
     <row r="21" spans="7:14">
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="25" spans="7:14">
       <c r="G25" s="5"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update SPI FLash part on BOM
</commit_message>
<xml_diff>
--- a/v2/BOM/bluzDK_bom.xlsx
+++ b/v2/BOM/bluzDK_bom.xlsx
@@ -114,9 +114,6 @@
     <t>2Mb SPI Flash</t>
   </si>
   <si>
-    <t>SST25VF020-20-4I-SAE</t>
-  </si>
-  <si>
     <t>ABS06-32.768KHZ-9-T</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>MCP1700T-3302E/TT</t>
+  </si>
+  <si>
+    <t>SST25VF020B-80-4I-SAE</t>
   </si>
 </sst>
 </file>
@@ -291,9 +291,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -332,7 +333,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -349,6 +350,7 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -682,7 +684,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -704,10 +706,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
@@ -716,16 +718,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -737,7 +739,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
@@ -750,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>3</v>
@@ -767,10 +769,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>30</v>
@@ -779,10 +781,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>3</v>
@@ -799,20 +801,20 @@
         <v>13</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>57</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>3</v>
@@ -830,7 +832,7 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>15</v>
@@ -840,7 +842,7 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>3</v>
@@ -857,10 +859,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>18</v>
@@ -884,13 +886,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>18</v>
@@ -900,7 +902,7 @@
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>3</v>
@@ -917,10 +919,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>18</v>
@@ -947,10 +949,10 @@
         <v>26</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>10</v>
@@ -977,11 +979,11 @@
         <v>21</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="11">
         <v>2</v>
@@ -1005,11 +1007,11 @@
         <v>23</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="11">
         <v>1</v>
@@ -1033,7 +1035,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
@@ -1061,7 +1063,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">

</xml_diff>

<commit_message>
updated RGB LED to new part. changed resistors for new LED. updated labeling on bluz.
</commit_message>
<xml_diff>
--- a/v2/BOM/bluzDK_bom.xlsx
+++ b/v2/BOM/bluzDK_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>Description</t>
   </si>
@@ -99,9 +99,6 @@
     <t>L2</t>
   </si>
   <si>
-    <t>R1-R6</t>
-  </si>
-  <si>
     <t>JP1, JP2</t>
   </si>
   <si>
@@ -193,6 +190,27 @@
   </si>
   <si>
     <t>SST25VF020B-80-4I-SAE</t>
+  </si>
+  <si>
+    <t>R1-R3</t>
+  </si>
+  <si>
+    <t>4.7k Ohm</t>
+  </si>
+  <si>
+    <t>10k Ohm</t>
+  </si>
+  <si>
+    <t>R4-R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>CRCW06034K70JNEA</t>
+  </si>
+  <si>
+    <t>CRCW060310K0FKEA</t>
   </si>
 </sst>
 </file>
@@ -208,7 +226,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -291,9 +308,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,7 +352,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -351,6 +370,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -681,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -706,10 +727,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
@@ -718,16 +739,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -739,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
@@ -752,7 +773,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>3</v>
@@ -769,22 +790,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>3</v>
@@ -801,20 +822,20 @@
         <v>13</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>3</v>
@@ -832,7 +853,7 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>15</v>
@@ -842,7 +863,7 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>3</v>
@@ -859,10 +880,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>18</v>
@@ -886,13 +907,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>18</v>
@@ -902,7 +923,7 @@
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>3</v>
@@ -919,10 +940,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>18</v>
@@ -946,23 +967,23 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="12" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>3</v>
@@ -976,77 +997,81 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="11"/>
+        <v>60</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="11" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E10" s="11">
         <v>2</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="12" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="K10" s="8"/>
       <c r="L10" s="7"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="D11" s="11" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E11" s="11">
         <v>1</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>3</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="7"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>45</v>
+        <v>21</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="E12" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="12" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>3</v>
@@ -1060,21 +1085,21 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E13" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>3</v>
@@ -1087,46 +1112,104 @@
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14">
+      <c r="A14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="11">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="J15"/>
-      <c r="K15"/>
-    </row>
-    <row r="20" spans="7:14" s="1" customFormat="1">
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="7:14">
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-    </row>
-    <row r="25" spans="7:14">
-      <c r="G25" s="5"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
+      <c r="A15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="11">
+        <v>2</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="7:14">
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="22" spans="7:14" s="1" customFormat="1">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="7:14">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="27" spans="7:14">
+      <c r="G27" s="5"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
     <hyperlink ref="H8" r:id="rId2"/>
     <hyperlink ref="H6" r:id="rId3"/>
-    <hyperlink ref="H10" r:id="rId4"/>
-    <hyperlink ref="H11" r:id="rId5"/>
-    <hyperlink ref="H12" r:id="rId6"/>
+    <hyperlink ref="H12" r:id="rId4"/>
+    <hyperlink ref="H13" r:id="rId5"/>
+    <hyperlink ref="H14" r:id="rId6"/>
     <hyperlink ref="H9" r:id="rId7"/>
-    <hyperlink ref="H13" r:id="rId8"/>
+    <hyperlink ref="H15" r:id="rId8"/>
     <hyperlink ref="H7" r:id="rId9"/>
     <hyperlink ref="H3" r:id="rId10"/>
     <hyperlink ref="H2" r:id="rId11"/>
     <hyperlink ref="H4" r:id="rId12"/>
+    <hyperlink ref="H10" r:id="rId13"/>
+    <hyperlink ref="H11" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updated BOM with correct RGB LED
</commit_message>
<xml_diff>
--- a/v2/BOM/bluzDK_bom.xlsx
+++ b/v2/BOM/bluzDK_bom.xlsx
@@ -93,9 +93,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>597-7701-207F</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>CRCW060310K0FKEA</t>
+  </si>
+  <si>
+    <t>CLVBA-FKA-CAEDH8BBB7A363</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -727,10 +727,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
@@ -739,16 +739,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -760,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
@@ -773,7 +773,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>3</v>
@@ -790,22 +790,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>3</v>
@@ -822,20 +822,20 @@
         <v>13</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>54</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>3</v>
@@ -853,7 +853,7 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>15</v>
@@ -863,7 +863,7 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>3</v>
@@ -880,10 +880,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>18</v>
@@ -907,13 +907,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>18</v>
@@ -923,7 +923,7 @@
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>3</v>
@@ -940,10 +940,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>18</v>
@@ -967,23 +967,23 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>58</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="11">
         <v>3</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>3</v>
@@ -997,13 +997,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>10</v>
@@ -1027,23 +1027,23 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="11">
         <v>1</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>3</v>
@@ -1060,11 +1060,11 @@
         <v>21</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="11">
         <v>2</v>
@@ -1088,18 +1088,18 @@
         <v>23</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="11">
         <v>1</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>3</v>
@@ -1113,10 +1113,10 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -1141,21 +1141,21 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="11">
         <v>2</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
cleanup some naming mistakes. properly labeled all capacitors
</commit_message>
<xml_diff>
--- a/v2/BOM/bluzDK_bom.xlsx
+++ b/v2/BOM/bluzDK_bom.xlsx
@@ -69,12 +69,6 @@
     <t>20ppm, 9pF, 32.768KHz crystal</t>
   </si>
   <si>
-    <t>C1, C2, C3</t>
-  </si>
-  <si>
-    <t>C5, C6</t>
-  </si>
-  <si>
     <t>0603 Package</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>ABS06-32.768KHZ-9-T</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
     <t>CL10B105KP8NNNC</t>
   </si>
   <si>
@@ -211,6 +202,15 @@
   </si>
   <si>
     <t>CLVBA-FKA-CAEDH8BBB7A363</t>
+  </si>
+  <si>
+    <t>C1-C3</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>C4, C5</t>
   </si>
 </sst>
 </file>
@@ -308,7 +308,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -330,8 +330,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -351,8 +353,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -372,6 +375,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -705,7 +710,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -727,10 +732,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
@@ -739,16 +744,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -760,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
@@ -773,7 +778,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>3</v>
@@ -790,22 +795,22 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>3</v>
@@ -822,20 +827,20 @@
         <v>13</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>3</v>
@@ -853,7 +858,7 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>15</v>
@@ -863,7 +868,7 @@
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>3</v>
@@ -876,54 +881,54 @@
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="11">
-        <v>3</v>
-      </c>
-      <c r="F6" s="11"/>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12"/>
       <c r="G6" s="12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="6"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>3</v>
@@ -937,23 +942,23 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="11" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="11">
         <v>2</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>3</v>
@@ -967,23 +972,23 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E9" s="11">
         <v>3</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>3</v>
@@ -997,13 +1002,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>10</v>
@@ -1027,23 +1032,23 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E11" s="11">
         <v>1</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>3</v>
@@ -1057,21 +1062,21 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E12" s="11">
         <v>2</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>3</v>
@@ -1085,21 +1090,21 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E13" s="11">
         <v>1</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>3</v>
@@ -1113,10 +1118,10 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -1141,21 +1146,21 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="11">
         <v>2</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>3</v>
@@ -1198,18 +1203,18 @@
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
     <hyperlink ref="H8" r:id="rId2"/>
-    <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId3"/>
     <hyperlink ref="H12" r:id="rId4"/>
     <hyperlink ref="H13" r:id="rId5"/>
     <hyperlink ref="H14" r:id="rId6"/>
     <hyperlink ref="H9" r:id="rId7"/>
     <hyperlink ref="H15" r:id="rId8"/>
-    <hyperlink ref="H7" r:id="rId9"/>
-    <hyperlink ref="H3" r:id="rId10"/>
-    <hyperlink ref="H2" r:id="rId11"/>
-    <hyperlink ref="H4" r:id="rId12"/>
-    <hyperlink ref="H10" r:id="rId13"/>
-    <hyperlink ref="H11" r:id="rId14"/>
+    <hyperlink ref="H3" r:id="rId9"/>
+    <hyperlink ref="H2" r:id="rId10"/>
+    <hyperlink ref="H4" r:id="rId11"/>
+    <hyperlink ref="H10" r:id="rId12"/>
+    <hyperlink ref="H11" r:id="rId13"/>
+    <hyperlink ref="H6" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>